<commit_message>
modify user profit report template
</commit_message>
<xml_diff>
--- a/src/Presentation/CTM.Win/ReportTemplate/UserDailyProfitFlow/DayReport.xlsx
+++ b/src/Presentation/CTM.Win/ReportTemplate/UserDailyProfitFlow/DayReport.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-30" yWindow="1050" windowWidth="18825" windowHeight="6780" tabRatio="693"/>
@@ -11,12 +11,12 @@
     <sheet name="合计" sheetId="94" r:id="rId2"/>
     <sheet name="吕志远" sheetId="158" r:id="rId3"/>
     <sheet name="骆加" sheetId="159" r:id="rId4"/>
-    <sheet name="王一峰" sheetId="162" r:id="rId5"/>
+    <sheet name="雷豪" sheetId="162" r:id="rId5"/>
     <sheet name="徐琪" sheetId="191" r:id="rId6"/>
     <sheet name="王亚运" sheetId="197" r:id="rId7"/>
     <sheet name="王超骏" sheetId="198" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -440,19 +440,13 @@
               <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>短差</a:t>
+              <a:t>雷豪</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>-</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>王一峰</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
@@ -510,7 +504,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$U$33</c:f>
+              <c:f>雷豪!$U$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -565,7 +559,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -589,7 +585,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -673,7 +669,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$U$34:$U$65</c:f>
+              <c:f>雷豪!$U$34:$U$65</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="32"/>
@@ -761,7 +757,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$Q$33</c:f>
+              <c:f>雷豪!$Q$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -802,7 +798,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -886,7 +882,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$Q$34:$Q$65</c:f>
+              <c:f>雷豪!$Q$34:$Q$65</c:f>
               <c:numCache>
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="32"/>
@@ -904,8 +900,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="218041728"/>
-        <c:axId val="218064000"/>
+        <c:axId val="-665048288"/>
+        <c:axId val="-665056992"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -915,7 +911,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$R$33</c:f>
+              <c:f>雷豪!$R$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1064,7 +1060,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1148,7 +1144,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$R$34:$R$65</c:f>
+              <c:f>雷豪!$R$34:$R$65</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="32"/>
@@ -1162,7 +1158,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$V$33</c:f>
+              <c:f>雷豪!$V$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1252,7 +1248,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1336,7 +1332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$V$34:$V$65</c:f>
+              <c:f>雷豪!$V$34:$V$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1350,7 +1346,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$G$33</c:f>
+              <c:f>雷豪!$G$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1420,7 +1416,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1490,7 +1488,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1574,7 +1572,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$G$34:$G$65</c:f>
+              <c:f>雷豪!$G$34:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1663,7 +1661,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$E$33</c:f>
+              <c:f>雷豪!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1715,7 +1713,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1749,7 +1749,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$E$34:$E$65</c:f>
+              <c:f>雷豪!$E$34:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="32"/>
@@ -1843,8 +1843,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="218041728"/>
-        <c:axId val="218064000"/>
+        <c:axId val="-665048288"/>
+        <c:axId val="-665056992"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1854,7 +1854,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$H$33</c:f>
+              <c:f>雷豪!$H$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1918,7 +1918,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -1998,7 +2000,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$H$34:$H$65</c:f>
+              <c:f>雷豪!$H$34:$H$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2087,7 +2089,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$X$33</c:f>
+              <c:f>雷豪!$X$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2127,7 +2129,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2186,7 +2190,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$X$34:$X$65</c:f>
+              <c:f>雷豪!$X$34:$X$65</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2296,7 +2300,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$M$33</c:f>
+              <c:f>雷豪!$M$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2348,7 +2352,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -2417,7 +2423,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$M$34:$M$65</c:f>
+              <c:f>雷豪!$M$34:$M$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2527,7 +2533,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$F$33</c:f>
+              <c:f>雷豪!$F$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2599,7 +2605,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2633,7 +2641,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$F$34:$F$65</c:f>
+              <c:f>雷豪!$F$34:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2727,11 +2735,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="218071808"/>
-        <c:axId val="218065920"/>
+        <c:axId val="-665046656"/>
+        <c:axId val="-665051552"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="218041728"/>
+        <c:axId val="-665048288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2751,7 +2759,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218064000"/>
+        <c:crossAx val="-665056992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -2759,7 +2767,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="218064000"/>
+        <c:axId val="-665056992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2831,12 +2839,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218041728"/>
+        <c:crossAx val="-665048288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218065920"/>
+        <c:axId val="-665051552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2856,12 +2864,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218071808"/>
+        <c:crossAx val="-665046656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="218071808"/>
+        <c:axId val="-665046656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2870,7 +2878,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218065920"/>
+        <c:crossAx val="-665051552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3059,7 +3067,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3473,8 +3483,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="223013504"/>
-        <c:axId val="223093120"/>
+        <c:axId val="-662403152"/>
+        <c:axId val="-662410768"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -3989,7 +3999,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4306,7 +4318,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4424,8 +4438,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223013504"/>
-        <c:axId val="223093120"/>
+        <c:axId val="-662403152"/>
+        <c:axId val="-662410768"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -4499,7 +4513,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4708,7 +4724,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4929,7 +4947,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -5180,7 +5200,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5298,11 +5320,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223105024"/>
-        <c:axId val="223095040"/>
+        <c:axId val="-662402608"/>
+        <c:axId val="-662405872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223013504"/>
+        <c:axId val="-662403152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5322,7 +5344,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223093120"/>
+        <c:crossAx val="-662410768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -5330,7 +5352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223093120"/>
+        <c:axId val="-662410768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5402,12 +5424,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223013504"/>
+        <c:crossAx val="-662403152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223095040"/>
+        <c:axId val="-662405872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5427,12 +5449,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223105024"/>
+        <c:crossAx val="-662402608"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="223105024"/>
+        <c:axId val="-662402608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5441,7 +5463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223095040"/>
+        <c:crossAx val="-662405872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5517,7 +5539,7 @@
               <a:rPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
-              <a:t>王一峰</a:t>
+              <a:t>雷豪</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
@@ -5575,7 +5597,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$U$33</c:f>
+              <c:f>雷豪!$U$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5630,7 +5652,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -5654,7 +5678,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -5738,7 +5762,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$U$34:$U$65</c:f>
+              <c:f>雷豪!$U$34:$U$65</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="32"/>
@@ -5826,7 +5850,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$Q$33</c:f>
+              <c:f>雷豪!$Q$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5867,7 +5891,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -5951,7 +5975,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$Q$34:$Q$65</c:f>
+              <c:f>雷豪!$Q$34:$Q$65</c:f>
               <c:numCache>
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="32"/>
@@ -5969,8 +5993,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="223349760"/>
-        <c:axId val="223372032"/>
+        <c:axId val="-662409680"/>
+        <c:axId val="-662409136"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -5980,7 +6004,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$R$33</c:f>
+              <c:f>雷豪!$R$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6129,7 +6153,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6213,7 +6237,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$R$34:$R$65</c:f>
+              <c:f>雷豪!$R$34:$R$65</c:f>
               <c:numCache>
                 <c:formatCode>_ * #,##0.0_ ;_ * \-#,##0.0_ ;_ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="32"/>
@@ -6227,7 +6251,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$V$33</c:f>
+              <c:f>雷豪!$V$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6317,7 +6341,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6401,7 +6425,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$V$34:$V$65</c:f>
+              <c:f>雷豪!$V$34:$V$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6415,7 +6439,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$G$33</c:f>
+              <c:f>雷豪!$G$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6485,7 +6509,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -6555,7 +6581,7 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>王一峰!$B$34:$B$65</c:f>
+              <c:f>雷豪!$B$34:$B$65</c:f>
               <c:numCache>
                 <c:formatCode>yy\/mm\/dd</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6639,7 +6665,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$G$34:$G$65</c:f>
+              <c:f>雷豪!$G$34:$G$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6728,7 +6754,7 @@
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$E$33</c:f>
+              <c:f>雷豪!$E$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6797,7 +6823,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -6821,7 +6849,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$E$34:$E$65</c:f>
+              <c:f>雷豪!$E$34:$E$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="32"/>
@@ -6915,8 +6943,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223349760"/>
-        <c:axId val="223372032"/>
+        <c:axId val="-662409680"/>
+        <c:axId val="-662409136"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -6926,7 +6954,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$H$33</c:f>
+              <c:f>雷豪!$H$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6990,7 +7018,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7070,7 +7100,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$H$34:$H$65</c:f>
+              <c:f>雷豪!$H$34:$H$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -7159,7 +7189,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$X$33</c:f>
+              <c:f>雷豪!$X$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7199,7 +7229,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7258,7 +7290,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$X$34:$X$65</c:f>
+              <c:f>雷豪!$X$34:$X$65</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -7368,7 +7400,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$M$33</c:f>
+              <c:f>雷豪!$M$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7420,7 +7452,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -7489,7 +7523,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$M$34:$M$65</c:f>
+              <c:f>雷豪!$M$34:$M$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -7599,7 +7633,7 @@
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>王一峰!$F$33</c:f>
+              <c:f>雷豪!$F$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7671,7 +7705,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -7695,7 +7731,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>王一峰!$F$34:$F$65</c:f>
+              <c:f>雷豪!$F$34:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="32"/>
@@ -7789,11 +7825,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223388032"/>
-        <c:axId val="223373952"/>
+        <c:axId val="-662408592"/>
+        <c:axId val="-662411312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223349760"/>
+        <c:axId val="-662409680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7813,7 +7849,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223372032"/>
+        <c:crossAx val="-662409136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -7821,7 +7857,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223372032"/>
+        <c:axId val="-662409136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7893,12 +7929,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223349760"/>
+        <c:crossAx val="-662409680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223373952"/>
+        <c:axId val="-662411312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7918,12 +7954,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223388032"/>
+        <c:crossAx val="-662408592"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="223388032"/>
+        <c:axId val="-662408592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7932,7 +7968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223373952"/>
+        <c:crossAx val="-662411312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8121,7 +8157,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -8535,8 +8573,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="223531392"/>
-        <c:axId val="223532928"/>
+        <c:axId val="-662411856"/>
+        <c:axId val="-662415120"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9051,7 +9089,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9368,7 +9408,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -9486,8 +9528,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223531392"/>
-        <c:axId val="223532928"/>
+        <c:axId val="-662411856"/>
+        <c:axId val="-662415120"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -9561,7 +9603,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9770,7 +9814,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -9991,7 +10037,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -10242,7 +10290,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -10360,11 +10410,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="223565312"/>
-        <c:axId val="223563776"/>
+        <c:axId val="-662405328"/>
+        <c:axId val="-662406416"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="223531392"/>
+        <c:axId val="-662411856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10384,7 +10434,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223532928"/>
+        <c:crossAx val="-662415120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -10392,7 +10442,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="223532928"/>
+        <c:axId val="-662415120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10464,12 +10514,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223531392"/>
+        <c:crossAx val="-662411856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="223563776"/>
+        <c:axId val="-662406416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10489,12 +10539,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="223565312"/>
+        <c:crossAx val="-662405328"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="223565312"/>
+        <c:axId val="-662405328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10503,7 +10553,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="223563776"/>
+        <c:crossAx val="-662406416"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10692,9 +10742,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -11108,8 +11156,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="224073216"/>
-        <c:axId val="224074752"/>
+        <c:axId val="-660341408"/>
+        <c:axId val="-660329440"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12059,8 +12107,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224073216"/>
-        <c:axId val="224074752"/>
+        <c:axId val="-660341408"/>
+        <c:axId val="-660329440"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -12343,9 +12391,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12566,9 +12612,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -12937,11 +12981,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="224098944"/>
-        <c:axId val="224097408"/>
+        <c:axId val="-660344128"/>
+        <c:axId val="-660344672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="224073216"/>
+        <c:axId val="-660341408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12961,7 +13005,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224074752"/>
+        <c:crossAx val="-660329440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -12969,7 +13013,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="224074752"/>
+        <c:axId val="-660329440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13041,12 +13085,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224073216"/>
+        <c:crossAx val="-660341408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="224097408"/>
+        <c:axId val="-660344672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13066,12 +13110,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="224098944"/>
+        <c:crossAx val="-660344128"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="224098944"/>
+        <c:axId val="-660344128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13080,7 +13124,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="224097408"/>
+        <c:crossAx val="-660344672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13269,9 +13313,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -13685,8 +13727,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="243059328"/>
-        <c:axId val="243093888"/>
+        <c:axId val="-660333248"/>
+        <c:axId val="-660343584"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14636,8 +14678,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243059328"/>
-        <c:axId val="243093888"/>
+        <c:axId val="-660333248"/>
+        <c:axId val="-660343584"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -14920,9 +14962,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -15143,9 +15183,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -15514,11 +15552,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="243097600"/>
-        <c:axId val="243095808"/>
+        <c:axId val="-660331072"/>
+        <c:axId val="-660335424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="243059328"/>
+        <c:axId val="-660333248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15538,7 +15576,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243093888"/>
+        <c:crossAx val="-660343584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -15546,7 +15584,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="243093888"/>
+        <c:axId val="-660343584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15618,12 +15656,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243059328"/>
+        <c:crossAx val="-660333248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="243095808"/>
+        <c:axId val="-660335424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15643,12 +15681,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="243097600"/>
+        <c:crossAx val="-660331072"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="243097600"/>
+        <c:axId val="-660331072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15657,7 +15695,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="243095808"/>
+        <c:crossAx val="-660335424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15736,6 +15774,12 @@
               <a:t>徐琪</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
@@ -15846,7 +15890,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -16047,8 +16093,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="218208512"/>
-        <c:axId val="218226688"/>
+        <c:axId val="-665049920"/>
+        <c:axId val="-665048832"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -16563,7 +16609,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -16875,7 +16923,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -17003,8 +17053,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="218208512"/>
-        <c:axId val="218226688"/>
+        <c:axId val="-665049920"/>
+        <c:axId val="-665048832"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -17078,7 +17128,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -17287,7 +17339,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -17508,7 +17562,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -17759,7 +17815,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -17887,11 +17945,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="218230144"/>
-        <c:axId val="218228608"/>
+        <c:axId val="-665047744"/>
+        <c:axId val="-665046112"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="218208512"/>
+        <c:axId val="-665049920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17911,7 +17969,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218226688"/>
+        <c:crossAx val="-665048832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -17919,7 +17977,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="218226688"/>
+        <c:axId val="-665048832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17991,12 +18049,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218208512"/>
+        <c:crossAx val="-665049920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218228608"/>
+        <c:axId val="-665046112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18016,12 +18074,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218230144"/>
+        <c:crossAx val="-665047744"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="218230144"/>
+        <c:axId val="-665047744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -18030,7 +18088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="218228608"/>
+        <c:crossAx val="-665046112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -18109,6 +18167,12 @@
               <a:t>骆加</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
@@ -18219,7 +18283,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -18633,8 +18699,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="221060096"/>
-        <c:axId val="221078272"/>
+        <c:axId val="-665043392"/>
+        <c:axId val="-665055360"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -19149,7 +19215,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -19466,7 +19534,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -19594,8 +19664,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221060096"/>
-        <c:axId val="221078272"/>
+        <c:axId val="-665043392"/>
+        <c:axId val="-665055360"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -19669,7 +19739,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -19878,7 +19950,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -20099,7 +20173,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -20350,7 +20426,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -20478,11 +20556,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221086080"/>
-        <c:axId val="221080192"/>
+        <c:axId val="-665051008"/>
+        <c:axId val="-665055904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221060096"/>
+        <c:axId val="-665043392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20502,7 +20580,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221078272"/>
+        <c:crossAx val="-665055360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -20510,7 +20588,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221078272"/>
+        <c:axId val="-665055360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20582,12 +20660,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221060096"/>
+        <c:crossAx val="-665043392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221080192"/>
+        <c:axId val="-665055904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20607,12 +20685,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221086080"/>
+        <c:crossAx val="-665051008"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="221086080"/>
+        <c:axId val="-665051008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -20621,7 +20699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221080192"/>
+        <c:crossAx val="-665055904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -20700,6 +20778,12 @@
               <a:t>吕志远</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
@@ -20810,7 +20894,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -21021,8 +21107,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="221817088"/>
-        <c:axId val="221843456"/>
+        <c:axId val="-665050464"/>
+        <c:axId val="-665052096"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -21537,7 +21623,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -21849,7 +21937,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -21977,8 +22067,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221817088"/>
-        <c:axId val="221843456"/>
+        <c:axId val="-665050464"/>
+        <c:axId val="-665052096"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -22052,7 +22142,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -22261,7 +22353,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -22482,7 +22576,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -22733,7 +22829,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -22861,11 +22959,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221846912"/>
-        <c:axId val="221845376"/>
+        <c:axId val="-665049376"/>
+        <c:axId val="-665042848"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221817088"/>
+        <c:axId val="-665050464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22885,7 +22983,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221843456"/>
+        <c:crossAx val="-665052096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -22893,7 +22991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221843456"/>
+        <c:axId val="-665052096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22965,12 +23063,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221817088"/>
+        <c:crossAx val="-665050464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221845376"/>
+        <c:axId val="-665042848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -22990,12 +23088,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221846912"/>
+        <c:crossAx val="-665049376"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="221846912"/>
+        <c:axId val="-665049376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -23004,7 +23102,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221845376"/>
+        <c:crossAx val="-665042848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -23083,6 +23181,12 @@
               <a:t>王亚运</a:t>
             </a:r>
             <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-</a:t>
+            </a:r>
+            <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
@@ -23193,7 +23297,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -23617,8 +23723,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="222447872"/>
-        <c:axId val="222486528"/>
+        <c:axId val="-665044480"/>
+        <c:axId val="-665043936"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -24133,7 +24239,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -24445,7 +24553,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -24573,8 +24683,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222447872"/>
-        <c:axId val="222486528"/>
+        <c:axId val="-665044480"/>
+        <c:axId val="-665043936"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -24648,7 +24758,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -24857,7 +24969,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -25078,7 +25192,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -25329,7 +25445,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -25457,11 +25575,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222489984"/>
-        <c:axId val="222488448"/>
+        <c:axId val="-665057536"/>
+        <c:axId val="-665042304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222447872"/>
+        <c:axId val="-665044480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25481,7 +25599,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222486528"/>
+        <c:crossAx val="-665043936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -25489,7 +25607,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222486528"/>
+        <c:axId val="-665043936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25561,12 +25679,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222447872"/>
+        <c:crossAx val="-665044480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222488448"/>
+        <c:axId val="-665042304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25586,12 +25704,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222489984"/>
+        <c:crossAx val="-665057536"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="222489984"/>
+        <c:axId val="-665057536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -25600,7 +25718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222488448"/>
+        <c:crossAx val="-665042304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -25677,6 +25795,12 @@
                 <a:effectLst/>
               </a:rPr>
               <a:t>王超骏</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>-</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="zh-CN" altLang="zh-CN" sz="1800" b="1" i="0" baseline="0">
@@ -26205,8 +26329,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="222869760"/>
-        <c:axId val="222629888"/>
+        <c:axId val="-663801216"/>
+        <c:axId val="-663805024"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -26721,7 +26845,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -27033,7 +27159,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -27151,8 +27279,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222869760"/>
-        <c:axId val="222629888"/>
+        <c:axId val="-663801216"/>
+        <c:axId val="-663805024"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -27226,7 +27354,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -27911,7 +28041,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -28029,11 +28161,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222633344"/>
-        <c:axId val="222631808"/>
+        <c:axId val="-663806656"/>
+        <c:axId val="-663803392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222869760"/>
+        <c:axId val="-663801216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28053,7 +28185,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222629888"/>
+        <c:crossAx val="-663805024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -28061,7 +28193,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222629888"/>
+        <c:axId val="-663805024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28133,12 +28265,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222869760"/>
+        <c:crossAx val="-663801216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222631808"/>
+        <c:axId val="-663803392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28158,12 +28290,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222633344"/>
+        <c:crossAx val="-663806656"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="222633344"/>
+        <c:axId val="-663806656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -28172,7 +28304,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222631808"/>
+        <c:crossAx val="-663803392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -28355,7 +28487,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -28769,8 +28903,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="332985088"/>
-        <c:axId val="332986624"/>
+        <c:axId val="-663806112"/>
+        <c:axId val="-663804480"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -28850,7 +28984,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -29162,7 +29298,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -29280,8 +29418,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="332985088"/>
-        <c:axId val="332986624"/>
+        <c:axId val="-663806112"/>
+        <c:axId val="-663804480"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -29355,7 +29493,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -29564,7 +29704,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -29785,7 +29927,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -30036,7 +30180,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -30154,11 +30300,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="333211520"/>
-        <c:axId val="333209984"/>
+        <c:axId val="-663803936"/>
+        <c:axId val="-663800672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="332985088"/>
+        <c:axId val="-663806112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30178,7 +30324,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332986624"/>
+        <c:crossAx val="-663804480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -30186,7 +30332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="332986624"/>
+        <c:axId val="-663804480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30258,12 +30404,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="332985088"/>
+        <c:crossAx val="-663806112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="333209984"/>
+        <c:axId val="-663800672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30283,12 +30429,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="333211520"/>
+        <c:crossAx val="-663803936"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="333211520"/>
+        <c:axId val="-663803936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -30297,7 +30443,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="333209984"/>
+        <c:crossAx val="-663800672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -30894,8 +31040,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="221514752"/>
-        <c:axId val="221532928"/>
+        <c:axId val="-663799584"/>
+        <c:axId val="-662410224"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -31405,8 +31551,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221514752"/>
-        <c:axId val="221532928"/>
+        <c:axId val="-663799584"/>
+        <c:axId val="-662410224"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -32279,11 +32425,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="221548928"/>
-        <c:axId val="221534848"/>
+        <c:axId val="-662412944"/>
+        <c:axId val="-662416208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="221514752"/>
+        <c:axId val="-663799584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -32303,7 +32449,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221532928"/>
+        <c:crossAx val="-662410224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -32311,7 +32457,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="221532928"/>
+        <c:axId val="-662410224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -32383,12 +32529,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221514752"/>
+        <c:crossAx val="-663799584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="221534848"/>
+        <c:axId val="-662416208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -32408,12 +32554,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="221548928"/>
+        <c:crossAx val="-662412944"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="221548928"/>
+        <c:axId val="-662412944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -32422,7 +32568,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="221534848"/>
+        <c:crossAx val="-662416208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -32611,7 +32757,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -32812,8 +32960,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="-68"/>
-        <c:axId val="222782976"/>
-        <c:axId val="222784512"/>
+        <c:axId val="-662406960"/>
+        <c:axId val="-662407504"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -33140,7 +33288,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -33457,7 +33607,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -33575,8 +33727,8 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222782976"/>
-        <c:axId val="222784512"/>
+        <c:axId val="-662406960"/>
+        <c:axId val="-662407504"/>
       </c:lineChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -33650,7 +33802,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -33859,7 +34013,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -34080,7 +34236,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -34331,7 +34489,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -34449,11 +34609,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="222800512"/>
-        <c:axId val="222798976"/>
+        <c:axId val="-662414032"/>
+        <c:axId val="-662404784"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="222782976"/>
+        <c:axId val="-662406960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34473,7 +34633,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222784512"/>
+        <c:crossAx val="-662407504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -34481,7 +34641,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="222784512"/>
+        <c:axId val="-662407504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34553,12 +34713,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222782976"/>
+        <c:crossAx val="-662406960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222798976"/>
+        <c:axId val="-662404784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34578,12 +34738,12 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222800512"/>
+        <c:crossAx val="-662414032"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="222800512"/>
+        <c:axId val="-662414032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -34592,7 +34752,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="222798976"/>
+        <c:crossAx val="-662404784"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -36451,7 +36611,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -36493,7 +36653,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -36528,7 +36688,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -36740,8 +36900,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="M13:M55"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A235" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Q234" sqref="Q234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -40857,7 +41017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y65"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L60" sqref="L60"/>
     </sheetView>
   </sheetViews>
@@ -42880,7 +43040,7 @@
   <dimension ref="A2:Y65"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1" x14ac:dyDescent="0.15"/>
@@ -44825,7 +44985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y65"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L61" sqref="L61"/>
     </sheetView>
   </sheetViews>

</xml_diff>